<commit_message>
suavizamiento exponencial de holt
</commit_message>
<xml_diff>
--- a/data/ses_holt_hw.xlsx
+++ b/data/ses_holt_hw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cod\MUSE_JCE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F784C3-A17F-4E52-9390-28C263F6E0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6ACED4-6F9B-46A5-8B24-F03595DDFD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-885" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{5CC513FC-EFB3-4569-9109-644D88F7E97D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{5CC513FC-EFB3-4569-9109-644D88F7E97D}"/>
   </bookViews>
   <sheets>
     <sheet name="SES" sheetId="3" r:id="rId1"/>
@@ -18,16 +18,22 @@
     <sheet name="Holt_winter" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Holt!$I$1:$I$2</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">Holt_winter!$I$1:$I$3,Holt_winter!$F$14:$F$17,Holt_winter!$D$17:$E$17</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">SES!$H$1,SES!$D$8</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">Holt_winter!$I$1</definedName>
@@ -38,26 +44,37 @@
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">Holt_winter!$I$2</definedName>
     <definedName name="solver_lhs5" localSheetId="2" hidden="1">Holt_winter!$I$3</definedName>
     <definedName name="solver_lhs6" localSheetId="2" hidden="1">Holt_winter!$I$3</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">6</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Holt!$G$4</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">Holt_winter!$G$6</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">SES!$F$2</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
@@ -76,24 +93,34 @@
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rhs6" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
@@ -116,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>Observation</t>
   </si>
@@ -234,16 +261,23 @@
       <t>t</t>
     </r>
   </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>PAE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -473,7 +507,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,9 +611,6 @@
     <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -654,6 +685,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -995,16 +1035,16 @@
                   <c:v>56688.250758078517</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>56688.250758078517</c:v>
+                  <c:v>17006.475227423558</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>56688.250758078517</c:v>
+                  <c:v>5101.9425682270685</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>56688.250758078517</c:v>
+                  <c:v>1530.5827704681208</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>56688.250758078517</c:v>
+                  <c:v>459.17483114043631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1280,6 +1320,102 @@
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>21.86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.745720955187394</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.23057877616214</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.246992389649765</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.020993373837047</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.837065011987224</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.148738254864654</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.176891919412043</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32.809001565540783</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.743810181436601</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.626222119352377</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.593520200614172</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34.481628586301639</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40.120149808510128</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43.395873852855679</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43.802259924663005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46.539923216502423</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>49.00561224897767</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50.857101232010407</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>53.580923191240771</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>52.148383307259408</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>62.301222685008675</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>66.680971536133924</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>69.875906499888046</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>71.609794963859684</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>71.115235862122901</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>72.069263494967387</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>74.646768539851294</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>76.795518809894617</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>78.944269079937953</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>81.09301934998129</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>83.241769620024613</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4268,8 +4404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15CC3305-0F10-4BFA-9234-5FFB9C915C1C}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4283,10 +4419,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="57"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="8" t="s">
         <v>7</v>
       </c>
@@ -4328,7 +4464,9 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -4425,7 +4563,7 @@
         <v>55691.635000000002</v>
       </c>
       <c r="D10" s="20">
-        <f t="shared" ref="D10:D35" si="0">$H$1*C9 +(1-$H$1)*D9</f>
+        <f t="shared" ref="D10:D39" si="0">$H$1*C9 +(1-$H$1)*D9</f>
         <v>42175.465196666672</v>
       </c>
       <c r="E10" s="21">
@@ -4517,7 +4655,7 @@
         <v>49633.199000000001</v>
       </c>
       <c r="D14" s="20">
-        <f t="shared" si="0"/>
+        <f>$H$1*C13 +(1-$H$1)*D13</f>
         <v>66694.996457592992</v>
       </c>
       <c r="E14" s="21">
@@ -4977,7 +5115,7 @@
         <v>60398.733</v>
       </c>
       <c r="D34" s="20">
-        <f t="shared" si="0"/>
+        <f>$H$1*C33 +(1-$H$1)*D33</f>
         <v>48030.458860261744</v>
       </c>
       <c r="E34" s="21">
@@ -5016,8 +5154,8 @@
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="20">
-        <f>$H$1*C34 +(1-$H$1)*D34</f>
-        <v>56688.250758078517</v>
+        <f t="shared" si="0"/>
+        <v>17006.475227423558</v>
       </c>
       <c r="E36" s="21">
         <v>2</v>
@@ -5034,8 +5172,8 @@
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="20">
-        <f>$H$1*C34 +(1-$H$1)*D34</f>
-        <v>56688.250758078517</v>
+        <f t="shared" si="0"/>
+        <v>5101.9425682270685</v>
       </c>
       <c r="E37" s="21">
         <v>3</v>
@@ -5052,8 +5190,8 @@
       </c>
       <c r="C38" s="23"/>
       <c r="D38" s="20">
-        <f>$H$1*C34 +(1-$H$1)*D34</f>
-        <v>56688.250758078517</v>
+        <f t="shared" si="0"/>
+        <v>1530.5827704681208</v>
       </c>
       <c r="E38" s="21">
         <v>4</v>
@@ -5070,8 +5208,8 @@
       </c>
       <c r="C39" s="23"/>
       <c r="D39" s="20">
-        <f>$H$1*C34 +(1-$H$1)*D34</f>
-        <v>56688.250758078517</v>
+        <f t="shared" si="0"/>
+        <v>459.17483114043631</v>
       </c>
       <c r="E39" s="21">
         <v>5</v>
@@ -5091,10 +5229,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C92A2A-80C6-4F2B-94A2-DE09EF091EAF}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5108,82 +5246,88 @@
     <col min="9" max="9" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F1" s="57" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F1" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="57"/>
+      <c r="G1" s="56"/>
       <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="9">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F2" s="58" t="s">
+        <v>0.80784866082320173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="59"/>
+      <c r="G2" s="58"/>
       <c r="H2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="9">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.27067718171280708</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="24"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="4">
-        <f>SUMPRODUCT(F11:F37,F11:F37)</f>
-        <v>0</v>
+        <f>SUMPRODUCT(H11:H39,H11:H39)</f>
+        <v>170.6599969991733</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4">
-        <f>G4/C37</f>
-        <v>0</v>
+      <c r="G5" s="64">
+        <f>G4/B39</f>
+        <v>6.320740629599011</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3">
         <f>SQRT(G5)</f>
-        <v>0</v>
+        <v>2.5141083169980982</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="3">
+        <f>AVERAGE(I13:I39)</f>
+        <v>1.6923140273157413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="6">
+        <f>AVERAGE(J13:J39)</f>
+        <v>4.4919855359310146E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>3</v>
       </c>
@@ -5210,7 +5354,7 @@
       </c>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
         <v>5</v>
@@ -5235,7 +5379,7 @@
       </c>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>1989</v>
       </c>
@@ -5243,7 +5387,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="18"/>
-      <c r="D12" s="56">
+      <c r="D12" s="55">
         <f>C13</f>
         <v>17.55</v>
       </c>
@@ -5254,8 +5398,14 @@
       <c r="F12" s="29"/>
       <c r="G12" s="15"/>
       <c r="H12" s="16"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>1990</v>
       </c>
@@ -5265,13 +5415,35 @@
       <c r="C13" s="30">
         <v>17.55</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="31">
+        <f>$I$1*C13+(1-$I$1)*(D12+E12)</f>
+        <v>18.378172271852002</v>
+      </c>
+      <c r="E13" s="32">
+        <f>$I$2*(D13-D12)+(1-$I$2)*E12</f>
+        <v>3.3675486833353929</v>
+      </c>
+      <c r="F13" s="33">
+        <f>D12+(G13*E12)</f>
+        <v>21.86</v>
+      </c>
+      <c r="G13" s="21">
+        <v>1</v>
+      </c>
+      <c r="H13" s="16">
+        <f>C13-F13</f>
+        <v>-4.3099999999999987</v>
+      </c>
+      <c r="I13" s="7">
+        <f>ABS(H13)</f>
+        <v>4.3099999999999987</v>
+      </c>
+      <c r="J13">
+        <f>I13/C13</f>
+        <v>0.24558404558404551</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>1991</v>
       </c>
@@ -5281,13 +5453,35 @@
       <c r="C14" s="34">
         <v>21.86</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="31">
+        <f t="shared" ref="D14:D39" si="0">$I$1*C14+(1-$I$1)*(D13+E13)</f>
+        <v>21.838041128499412</v>
+      </c>
+      <c r="E14" s="32">
+        <f t="shared" ref="E14:E39" si="1">$I$2*(D14-D13)+(1-$I$2)*E13</f>
+        <v>3.3925376476627278</v>
+      </c>
+      <c r="F14" s="33">
+        <f t="shared" ref="F14:F40" si="2">D13+(G14*E13)</f>
+        <v>21.745720955187394</v>
+      </c>
+      <c r="G14" s="21">
+        <v>1</v>
+      </c>
+      <c r="H14" s="16">
+        <f t="shared" ref="H14:H44" si="3">C14-F14</f>
+        <v>0.11427904481260498</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" ref="I14:I44" si="4">ABS(H14)</f>
+        <v>0.11427904481260498</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14:J44" si="5">I14/C14</f>
+        <v>5.2277696620587821E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>1992</v>
       </c>
@@ -5297,13 +5491,35 @@
       <c r="C15" s="30">
         <v>23.89</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="16"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="31">
+        <f t="shared" si="0"/>
+        <v>24.147594007111547</v>
+      </c>
+      <c r="E15" s="32">
+        <f t="shared" si="1"/>
+        <v>3.0993983825382179</v>
+      </c>
+      <c r="F15" s="33">
+        <f t="shared" si="2"/>
+        <v>25.23057877616214</v>
+      </c>
+      <c r="G15" s="21">
+        <v>1</v>
+      </c>
+      <c r="H15" s="16">
+        <f t="shared" si="3"/>
+        <v>-1.3405787761621397</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="4"/>
+        <v>1.3405787761621397</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="5"/>
+        <v>5.6114641111851805E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>1993</v>
       </c>
@@ -5313,13 +5529,35 @@
       <c r="C16" s="34">
         <v>26.93</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="16"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="31">
+        <f t="shared" si="0"/>
+        <v>26.990910512180054</v>
+      </c>
+      <c r="E16" s="32">
+        <f t="shared" si="1"/>
+        <v>3.0300828616569921</v>
+      </c>
+      <c r="F16" s="33">
+        <f t="shared" si="2"/>
+        <v>27.246992389649765</v>
+      </c>
+      <c r="G16" s="21">
+        <v>1</v>
+      </c>
+      <c r="H16" s="16">
+        <f t="shared" si="3"/>
+        <v>-0.31699238964976573</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="4"/>
+        <v>0.31699238964976573</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>1.1770976221677153E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>1994</v>
       </c>
@@ -5329,13 +5567,35 @@
       <c r="C17" s="30">
         <v>26.89</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="31">
+        <f t="shared" si="0"/>
+        <v>27.491624569736469</v>
+      </c>
+      <c r="E17" s="32">
+        <f t="shared" si="1"/>
+        <v>2.3454404422507547</v>
+      </c>
+      <c r="F17" s="33">
+        <f t="shared" si="2"/>
+        <v>30.020993373837047</v>
+      </c>
+      <c r="G17" s="21">
+        <v>1</v>
+      </c>
+      <c r="H17" s="16">
+        <f t="shared" si="3"/>
+        <v>-3.1309933738370468</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="4"/>
+        <v>3.1309933738370468</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>0.11643709088274626</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>1995</v>
       </c>
@@ -5345,13 +5605,35 @@
       <c r="C18" s="34">
         <v>28.83</v>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="16"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="31">
+        <f t="shared" si="0"/>
+        <v>29.023508890691442</v>
+      </c>
+      <c r="E18" s="32">
+        <f t="shared" si="1"/>
+        <v>2.1252293641732098</v>
+      </c>
+      <c r="F18" s="33">
+        <f t="shared" si="2"/>
+        <v>29.837065011987224</v>
+      </c>
+      <c r="G18" s="21">
+        <v>1</v>
+      </c>
+      <c r="H18" s="16">
+        <f t="shared" si="3"/>
+        <v>-1.0070650119872262</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="4"/>
+        <v>1.0070650119872262</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="5"/>
+        <v>3.4931148525398067E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>1996</v>
       </c>
@@ -5361,13 +5643,35 @@
       <c r="C19" s="30">
         <v>30.08</v>
       </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="16"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="31">
+        <f t="shared" si="0"/>
+        <v>30.285359486901719</v>
+      </c>
+      <c r="E19" s="32">
+        <f t="shared" si="1"/>
+        <v>1.8915324325103273</v>
+      </c>
+      <c r="F19" s="33">
+        <f t="shared" si="2"/>
+        <v>31.148738254864654</v>
+      </c>
+      <c r="G19" s="21">
+        <v>1</v>
+      </c>
+      <c r="H19" s="16">
+        <f t="shared" si="3"/>
+        <v>-1.0687382548646553</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" si="4"/>
+        <v>1.0687382548646553</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>3.5529862196298383E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>1997</v>
       </c>
@@ -5377,13 +5681,35 @@
       <c r="C20" s="34">
         <v>30.95</v>
       </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D20" s="31">
+        <f t="shared" si="0"/>
+        <v>31.185748925340214</v>
+      </c>
+      <c r="E20" s="32">
+        <f t="shared" si="1"/>
+        <v>1.6232526402005703</v>
+      </c>
+      <c r="F20" s="33">
+        <f t="shared" si="2"/>
+        <v>32.176891919412043</v>
+      </c>
+      <c r="G20" s="21">
+        <v>1</v>
+      </c>
+      <c r="H20" s="16">
+        <f t="shared" si="3"/>
+        <v>-1.2268919194120436</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="4"/>
+        <v>1.2268919194120436</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>3.9641095942230808E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>1998</v>
       </c>
@@ -5393,13 +5719,35 @@
       <c r="C21" s="30">
         <v>30.19</v>
       </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="16"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="31">
+        <f t="shared" si="0"/>
+        <v>30.693244658124794</v>
+      </c>
+      <c r="E21" s="32">
+        <f t="shared" si="1"/>
+        <v>1.0505655233118054</v>
+      </c>
+      <c r="F21" s="33">
+        <f t="shared" si="2"/>
+        <v>32.809001565540783</v>
+      </c>
+      <c r="G21" s="21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="16">
+        <f t="shared" si="3"/>
+        <v>-2.6190015655407812</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="4"/>
+        <v>2.6190015655407812</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>8.6750631518409449E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>1999</v>
       </c>
@@ -5409,13 +5757,35 @@
       <c r="C22" s="34">
         <v>31.58</v>
       </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="16"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="31">
+        <f t="shared" si="0"/>
+        <v>31.611476345733838</v>
+      </c>
+      <c r="E22" s="32">
+        <f t="shared" si="1"/>
+        <v>1.0147457736185364</v>
+      </c>
+      <c r="F22" s="33">
+        <f t="shared" si="2"/>
+        <v>31.743810181436601</v>
+      </c>
+      <c r="G22" s="21">
+        <v>1</v>
+      </c>
+      <c r="H22" s="16">
+        <f t="shared" si="3"/>
+        <v>-0.16381018143660242</v>
+      </c>
+      <c r="I22" s="7">
+        <f t="shared" si="4"/>
+        <v>0.16381018143660242</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="5"/>
+        <v>5.1871495071755041E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>2000</v>
       </c>
@@ -5425,13 +5795,35 @@
       <c r="C23" s="30">
         <v>32.58</v>
       </c>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="31">
+        <f t="shared" si="0"/>
+        <v>32.588881642133146</v>
+      </c>
+      <c r="E23" s="32">
+        <f t="shared" si="1"/>
+        <v>1.0046385584810242</v>
+      </c>
+      <c r="F23" s="33">
+        <f t="shared" si="2"/>
+        <v>32.626222119352377</v>
+      </c>
+      <c r="G23" s="21">
+        <v>1</v>
+      </c>
+      <c r="H23" s="16">
+        <f t="shared" si="3"/>
+        <v>-4.6222119352378854E-2</v>
+      </c>
+      <c r="I23" s="7">
+        <f t="shared" si="4"/>
+        <v>4.6222119352378854E-2</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>1.4187268063959133E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>2001</v>
       </c>
@@ -5441,13 +5833,35 @@
       <c r="C24" s="34">
         <v>33.479999999999997</v>
       </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="16"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="31">
+        <f t="shared" si="0"/>
+        <v>33.501813058571628</v>
+      </c>
+      <c r="E24" s="32">
+        <f t="shared" si="1"/>
+        <v>0.9798155277300129</v>
+      </c>
+      <c r="F24" s="33">
+        <f t="shared" si="2"/>
+        <v>33.593520200614172</v>
+      </c>
+      <c r="G24" s="21">
+        <v>1</v>
+      </c>
+      <c r="H24" s="16">
+        <f t="shared" si="3"/>
+        <v>-0.11352020061417534</v>
+      </c>
+      <c r="I24" s="7">
+        <f t="shared" si="4"/>
+        <v>0.11352020061417534</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>3.3906869956444249E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>2002</v>
       </c>
@@ -5457,13 +5871,35 @@
       <c r="C25" s="30">
         <v>39.020000000000003</v>
       </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="16"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="31">
+        <f t="shared" si="0"/>
+        <v>38.147945855176161</v>
+      </c>
+      <c r="E25" s="32">
+        <f t="shared" si="1"/>
+        <v>1.9722039533339641</v>
+      </c>
+      <c r="F25" s="33">
+        <f t="shared" si="2"/>
+        <v>34.481628586301639</v>
+      </c>
+      <c r="G25" s="21">
+        <v>1</v>
+      </c>
+      <c r="H25" s="16">
+        <f t="shared" si="3"/>
+        <v>4.5383714136983642</v>
+      </c>
+      <c r="I25" s="7">
+        <f t="shared" si="4"/>
+        <v>4.5383714136983642</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="5"/>
+        <v>0.11630885222189553</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>2003</v>
       </c>
@@ -5473,13 +5909,35 @@
       <c r="C26" s="34">
         <v>41.39</v>
       </c>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="16"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="31">
+        <f t="shared" si="0"/>
+        <v>41.145996585151309</v>
+      </c>
+      <c r="E26" s="32">
+        <f t="shared" si="1"/>
+        <v>2.2498772677043672</v>
+      </c>
+      <c r="F26" s="33">
+        <f t="shared" si="2"/>
+        <v>40.120149808510128</v>
+      </c>
+      <c r="G26" s="21">
+        <v>1</v>
+      </c>
+      <c r="H26" s="16">
+        <f t="shared" si="3"/>
+        <v>1.2698501914898728</v>
+      </c>
+      <c r="I26" s="7">
+        <f t="shared" si="4"/>
+        <v>1.2698501914898728</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="5"/>
+        <v>3.0680120596517823E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>2004</v>
       </c>
@@ -5489,13 +5947,35 @@
       <c r="C27" s="30">
         <v>41.6</v>
       </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="16"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="31">
+        <f t="shared" si="0"/>
+        <v>41.945079565818816</v>
+      </c>
+      <c r="E27" s="32">
+        <f t="shared" si="1"/>
+        <v>1.8571803588441886</v>
+      </c>
+      <c r="F27" s="33">
+        <f t="shared" si="2"/>
+        <v>43.395873852855679</v>
+      </c>
+      <c r="G27" s="21">
+        <v>1</v>
+      </c>
+      <c r="H27" s="16">
+        <f t="shared" si="3"/>
+        <v>-1.7958738528556779</v>
+      </c>
+      <c r="I27" s="7">
+        <f t="shared" si="4"/>
+        <v>1.7958738528556779</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>4.3170044539799945E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>2005</v>
       </c>
@@ -5505,13 +5985,35 @@
       <c r="C28" s="34">
         <v>44.66</v>
       </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="16"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="31">
+        <f t="shared" si="0"/>
+        <v>44.495184095858384</v>
+      </c>
+      <c r="E28" s="32">
+        <f t="shared" si="1"/>
+        <v>2.0447391206440368</v>
+      </c>
+      <c r="F28" s="33">
+        <f t="shared" si="2"/>
+        <v>43.802259924663005</v>
+      </c>
+      <c r="G28" s="21">
+        <v>1</v>
+      </c>
+      <c r="H28" s="16">
+        <f t="shared" si="3"/>
+        <v>0.85774007533699148</v>
+      </c>
+      <c r="I28" s="7">
+        <f t="shared" si="4"/>
+        <v>0.85774007533699148</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>1.9206002582556909E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>2006</v>
       </c>
@@ -5521,13 +6023,35 @@
       <c r="C29" s="30">
         <v>46.95</v>
       </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="16"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="31">
+        <f t="shared" si="0"/>
+        <v>46.871203196885631</v>
+      </c>
+      <c r="E29" s="32">
+        <f t="shared" si="1"/>
+        <v>2.134409052092038</v>
+      </c>
+      <c r="F29" s="33">
+        <f t="shared" si="2"/>
+        <v>46.539923216502423</v>
+      </c>
+      <c r="G29" s="21">
+        <v>1</v>
+      </c>
+      <c r="H29" s="16">
+        <f t="shared" si="3"/>
+        <v>0.41007678349757981</v>
+      </c>
+      <c r="I29" s="7">
+        <f t="shared" si="4"/>
+        <v>0.41007678349757981</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>8.7343297869559057E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="18">
         <v>2007</v>
       </c>
@@ -5537,13 +6061,35 @@
       <c r="C30" s="34">
         <v>48.73</v>
       </c>
-      <c r="D30" s="31"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="16"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="31">
+        <f t="shared" si="0"/>
+        <v>48.782959262734586</v>
+      </c>
+      <c r="E30" s="32">
+        <f t="shared" si="1"/>
+        <v>2.0741419692758196</v>
+      </c>
+      <c r="F30" s="33">
+        <f t="shared" si="2"/>
+        <v>49.00561224897767</v>
+      </c>
+      <c r="G30" s="21">
+        <v>1</v>
+      </c>
+      <c r="H30" s="16">
+        <f t="shared" si="3"/>
+        <v>-0.27561224897767289</v>
+      </c>
+      <c r="I30" s="7">
+        <f t="shared" si="4"/>
+        <v>0.27561224897767289</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>5.6559049656817757E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>2008</v>
       </c>
@@ -5553,13 +6099,35 @@
       <c r="C31" s="30">
         <v>51.49</v>
       </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D31" s="31">
+        <f t="shared" si="0"/>
+        <v>51.368387654167456</v>
+      </c>
+      <c r="E31" s="32">
+        <f t="shared" si="1"/>
+        <v>2.2125355370733146</v>
+      </c>
+      <c r="F31" s="33">
+        <f t="shared" si="2"/>
+        <v>50.857101232010407</v>
+      </c>
+      <c r="G31" s="21">
+        <v>1</v>
+      </c>
+      <c r="H31" s="16">
+        <f t="shared" si="3"/>
+        <v>0.63289876798959455</v>
+      </c>
+      <c r="I31" s="7">
+        <f t="shared" si="4"/>
+        <v>0.63289876798959455</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="5"/>
+        <v>1.2291683200419392E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="18">
         <v>2009</v>
       </c>
@@ -5569,13 +6137,35 @@
       <c r="C32" s="34">
         <v>50.03</v>
       </c>
-      <c r="D32" s="31"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="16"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D32" s="31">
+        <f t="shared" si="0"/>
+        <v>50.712314646510862</v>
+      </c>
+      <c r="E32" s="32">
+        <f t="shared" si="1"/>
+        <v>1.4360686607485458</v>
+      </c>
+      <c r="F32" s="33">
+        <f t="shared" si="2"/>
+        <v>53.580923191240771</v>
+      </c>
+      <c r="G32" s="21">
+        <v>1</v>
+      </c>
+      <c r="H32" s="16">
+        <f t="shared" si="3"/>
+        <v>-3.5509231912407699</v>
+      </c>
+      <c r="I32" s="7">
+        <f t="shared" si="4"/>
+        <v>3.5509231912407699</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>7.0975878297836692E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>2010</v>
       </c>
@@ -5585,13 +6175,35 @@
       <c r="C33" s="30">
         <v>60.64</v>
       </c>
-      <c r="D33" s="31"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="16"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D33" s="31">
+        <f t="shared" si="0"/>
+        <v>59.008324480713839</v>
+      </c>
+      <c r="E33" s="32">
+        <f t="shared" si="1"/>
+        <v>3.292898204294838</v>
+      </c>
+      <c r="F33" s="33">
+        <f t="shared" si="2"/>
+        <v>52.148383307259408</v>
+      </c>
+      <c r="G33" s="21">
+        <v>1</v>
+      </c>
+      <c r="H33" s="16">
+        <f t="shared" si="3"/>
+        <v>8.4916166927405925</v>
+      </c>
+      <c r="I33" s="7">
+        <f t="shared" si="4"/>
+        <v>8.4916166927405925</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>0.14003325680640819</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="18">
         <v>2011</v>
       </c>
@@ -5601,13 +6213,35 @@
       <c r="C34" s="34">
         <v>63.36</v>
       </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="16"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="31">
+        <f t="shared" si="0"/>
+        <v>63.156554521034401</v>
+      </c>
+      <c r="E34" s="32">
+        <f t="shared" si="1"/>
+        <v>3.5244170150995222</v>
+      </c>
+      <c r="F34" s="33">
+        <f t="shared" si="2"/>
+        <v>62.301222685008675</v>
+      </c>
+      <c r="G34" s="21">
+        <v>1</v>
+      </c>
+      <c r="H34" s="16">
+        <f t="shared" si="3"/>
+        <v>1.0587773149913247</v>
+      </c>
+      <c r="I34" s="7">
+        <f t="shared" si="4"/>
+        <v>1.0587773149913247</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="5"/>
+        <v>1.6710500552262069E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>2012</v>
       </c>
@@ -5617,13 +6251,35 @@
       <c r="C35" s="30">
         <v>66.36</v>
       </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="16"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D35" s="31">
+        <f t="shared" si="0"/>
+        <v>66.42167511050576</v>
+      </c>
+      <c r="E35" s="32">
+        <f t="shared" si="1"/>
+        <v>3.454231389382286</v>
+      </c>
+      <c r="F35" s="33">
+        <f t="shared" si="2"/>
+        <v>66.680971536133924</v>
+      </c>
+      <c r="G35" s="21">
+        <v>1</v>
+      </c>
+      <c r="H35" s="16">
+        <f t="shared" si="3"/>
+        <v>-0.32097153613392493</v>
+      </c>
+      <c r="I35" s="7">
+        <f t="shared" si="4"/>
+        <v>0.32097153613392493</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="5"/>
+        <v>4.8368224251646311E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="18">
         <v>2013</v>
       </c>
@@ -5633,13 +6289,35 @@
       <c r="C36" s="34">
         <v>68.2</v>
       </c>
-      <c r="D36" s="31"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="16"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D36" s="31">
+        <f t="shared" si="0"/>
+        <v>68.522027678288595</v>
+      </c>
+      <c r="E36" s="32">
+        <f t="shared" si="1"/>
+        <v>3.0877672855710903</v>
+      </c>
+      <c r="F36" s="33">
+        <f t="shared" si="2"/>
+        <v>69.875906499888046</v>
+      </c>
+      <c r="G36" s="21">
+        <v>1</v>
+      </c>
+      <c r="H36" s="16">
+        <f t="shared" si="3"/>
+        <v>-1.6759064998880433</v>
+      </c>
+      <c r="I36" s="7">
+        <f t="shared" si="4"/>
+        <v>1.6759064998880433</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="5"/>
+        <v>2.4573409089267497E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>2014</v>
       </c>
@@ -5649,13 +6327,35 @@
       <c r="C37" s="30">
         <v>68.12</v>
       </c>
-      <c r="D37" s="31"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="16"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D37" s="31">
+        <f t="shared" si="0"/>
+        <v>68.790568775758089</v>
+      </c>
+      <c r="E37" s="32">
+        <f t="shared" si="1"/>
+        <v>2.3246670863648102</v>
+      </c>
+      <c r="F37" s="33">
+        <f t="shared" si="2"/>
+        <v>71.609794963859684</v>
+      </c>
+      <c r="G37" s="21">
+        <v>1</v>
+      </c>
+      <c r="H37" s="16">
+        <f t="shared" si="3"/>
+        <v>-3.4897949638596799</v>
+      </c>
+      <c r="I37" s="7">
+        <f t="shared" si="4"/>
+        <v>3.4897949638596799</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="5"/>
+        <v>5.1230108101287135E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
         <v>2015</v>
       </c>
@@ -5665,13 +6365,35 @@
       <c r="C38" s="34">
         <v>69.78</v>
       </c>
-      <c r="D38" s="31"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="16"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D38" s="31">
+        <f t="shared" si="0"/>
+        <v>70.036567359023806</v>
+      </c>
+      <c r="E38" s="32">
+        <f t="shared" si="1"/>
+        <v>2.0326961359435756</v>
+      </c>
+      <c r="F38" s="33">
+        <f t="shared" si="2"/>
+        <v>71.115235862122901</v>
+      </c>
+      <c r="G38" s="21">
+        <v>1</v>
+      </c>
+      <c r="H38" s="16">
+        <f t="shared" si="3"/>
+        <v>-1.3352358621229001</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="4"/>
+        <v>1.3352358621229001</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="5"/>
+        <v>1.9134936401875899E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>2016</v>
       </c>
@@ -5681,13 +6403,35 @@
       <c r="C39" s="30">
         <v>72.599999999999994</v>
       </c>
-      <c r="D39" s="31"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="16"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D39" s="31">
+        <f t="shared" si="0"/>
+        <v>72.498018269807957</v>
+      </c>
+      <c r="E39" s="32">
+        <f t="shared" si="1"/>
+        <v>2.1487502700433319</v>
+      </c>
+      <c r="F39" s="33">
+        <f t="shared" si="2"/>
+        <v>72.069263494967387</v>
+      </c>
+      <c r="G39" s="21">
+        <v>1</v>
+      </c>
+      <c r="H39" s="16">
+        <f t="shared" si="3"/>
+        <v>0.53073650503260694</v>
+      </c>
+      <c r="I39" s="7">
+        <f t="shared" si="4"/>
+        <v>0.53073650503260694</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="5"/>
+        <v>7.3104201795124932E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="22">
         <v>2017</v>
       </c>
@@ -5695,13 +6439,22 @@
         <v>28</v>
       </c>
       <c r="C40" s="22"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="15"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="33">
+        <f>$D$39+(G40*$E$39)</f>
+        <v>74.646768539851294</v>
+      </c>
+      <c r="G40" s="21">
+        <v>1</v>
+      </c>
       <c r="H40" s="16"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J40" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>2018</v>
       </c>
@@ -5711,11 +6464,20 @@
       <c r="C41" s="22"/>
       <c r="D41" s="35"/>
       <c r="E41" s="36"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="15"/>
+      <c r="F41" s="33">
+        <f>$D$39+(G41*$E$39)</f>
+        <v>76.795518809894617</v>
+      </c>
+      <c r="G41" s="62">
+        <v>2</v>
+      </c>
       <c r="H41" s="16"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J41" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="22">
         <v>2019</v>
       </c>
@@ -5725,11 +6487,20 @@
       <c r="C42" s="22"/>
       <c r="D42" s="35"/>
       <c r="E42" s="36"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="15"/>
+      <c r="F42" s="33">
+        <f>$D$39+(G42*$E$39)</f>
+        <v>78.944269079937953</v>
+      </c>
+      <c r="G42" s="62">
+        <v>3</v>
+      </c>
       <c r="H42" s="16"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J42" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>2020</v>
       </c>
@@ -5739,11 +6510,20 @@
       <c r="C43" s="22"/>
       <c r="D43" s="35"/>
       <c r="E43" s="36"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="15"/>
+      <c r="F43" s="33">
+        <f>$D$39+(G43*$E$39)</f>
+        <v>81.09301934998129</v>
+      </c>
+      <c r="G43" s="62">
+        <v>4</v>
+      </c>
       <c r="H43" s="16"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J43" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="22">
         <v>2021</v>
       </c>
@@ -5753,9 +6533,18 @@
       <c r="C44" s="22"/>
       <c r="D44" s="35"/>
       <c r="E44" s="36"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="21"/>
+      <c r="F44" s="33">
+        <f t="shared" ref="F41:F44" si="6">$D$39+(G44*$E$39)</f>
+        <v>83.241769620024613</v>
+      </c>
+      <c r="G44" s="63">
+        <v>5</v>
+      </c>
+      <c r="H44" s="16"/>
+      <c r="J44" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5771,8 +6560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7883B9A0-6EC6-4601-BFF4-342B674DDDB4}">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51:B54"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5791,38 +6580,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="38" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="39">
+      <c r="I1" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="38" t="s">
+      <c r="G2" s="58"/>
+      <c r="H2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="39">
+      <c r="I2" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="38" t="s">
+      <c r="G3" s="58"/>
+      <c r="H3" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="39">
+      <c r="I3" s="38">
         <v>1</v>
       </c>
     </row>
@@ -5837,10 +6626,10 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="59"/>
+      <c r="G5" s="58"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
     </row>
@@ -5917,7 +6706,7 @@
       <c r="I12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="40" t="s">
+      <c r="J12" s="39" t="s">
         <v>32</v>
       </c>
       <c r="K12" s="8" t="s">
@@ -5954,7 +6743,7 @@
       <c r="I13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="40"/>
+      <c r="J13" s="39"/>
       <c r="K13" s="21"/>
       <c r="L13" s="15"/>
       <c r="M13" s="21"/>
@@ -5968,14 +6757,14 @@
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="42">
+      <c r="E14" s="40"/>
+      <c r="F14" s="41">
         <v>0</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="40"/>
+      <c r="J14" s="39"/>
       <c r="K14" s="21"/>
       <c r="L14" s="15"/>
       <c r="M14" s="21"/>
@@ -5989,14 +6778,14 @@
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42">
+      <c r="E15" s="40"/>
+      <c r="F15" s="41">
         <v>17.532009494090538</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="40"/>
+      <c r="J15" s="39"/>
       <c r="K15" s="21"/>
       <c r="L15" s="15"/>
       <c r="M15" s="21"/>
@@ -6010,14 +6799,14 @@
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="42">
+      <c r="E16" s="40"/>
+      <c r="F16" s="41">
         <v>15.820255942810377</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="40"/>
+      <c r="J16" s="39"/>
       <c r="K16" s="21"/>
       <c r="L16" s="15"/>
       <c r="M16" s="21"/>
@@ -6036,10 +6825,10 @@
       <c r="E17" s="28">
         <v>2.2557485084678475</v>
       </c>
-      <c r="F17" s="42">
+      <c r="F17" s="41">
         <v>59.912706402693409</v>
       </c>
-      <c r="G17" s="43"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="15"/>
       <c r="I17" s="16"/>
       <c r="J17" s="21"/>
@@ -6185,7 +6974,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="21">
-        <f t="shared" ref="K20:K63" si="8">$G$4*(J20+1)</f>
+        <f t="shared" ref="K20:K62" si="8">$G$4*(J20+1)</f>
         <v>4</v>
       </c>
       <c r="L20" s="21">
@@ -7425,10 +8214,10 @@
         <f t="shared" si="9"/>
         <v>1974</v>
       </c>
-      <c r="B45" s="44">
+      <c r="B45" s="43">
         <v>28</v>
       </c>
-      <c r="C45" s="44">
+      <c r="C45" s="43">
         <v>228.21700000000001</v>
       </c>
       <c r="D45" s="31">
@@ -7476,10 +8265,10 @@
         <f t="shared" si="9"/>
         <v>1974</v>
       </c>
-      <c r="B46" s="44">
+      <c r="B46" s="43">
         <v>29</v>
       </c>
-      <c r="C46" s="44">
+      <c r="C46" s="43">
         <v>124.387</v>
       </c>
       <c r="D46" s="31">
@@ -7527,10 +8316,10 @@
         <f t="shared" si="9"/>
         <v>1975</v>
       </c>
-      <c r="B47" s="44">
+      <c r="B47" s="43">
         <v>30</v>
       </c>
-      <c r="C47" s="44">
+      <c r="C47" s="43">
         <v>138.79</v>
       </c>
       <c r="D47" s="31">
@@ -7578,10 +8367,10 @@
         <f t="shared" si="9"/>
         <v>1975</v>
       </c>
-      <c r="B48" s="44">
+      <c r="B48" s="43">
         <v>31</v>
       </c>
-      <c r="C48" s="44">
+      <c r="C48" s="43">
         <v>145.12200000000001</v>
       </c>
       <c r="D48" s="31">
@@ -7629,10 +8418,10 @@
         <f t="shared" si="9"/>
         <v>1975</v>
       </c>
-      <c r="B49" s="44">
+      <c r="B49" s="43">
         <v>32</v>
       </c>
-      <c r="C49" s="44">
+      <c r="C49" s="43">
         <v>233.429</v>
       </c>
       <c r="D49" s="31">
@@ -7680,7 +8469,7 @@
         <f t="shared" si="9"/>
         <v>1975</v>
       </c>
-      <c r="B50" s="44">
+      <c r="B50" s="43">
         <v>33</v>
       </c>
       <c r="C50" s="21">
@@ -7731,7 +8520,7 @@
         <f t="shared" si="9"/>
         <v>1976</v>
       </c>
-      <c r="B51" s="44">
+      <c r="B51" s="43">
         <v>34</v>
       </c>
       <c r="C51" s="21">
@@ -7782,7 +8571,7 @@
         <f t="shared" si="9"/>
         <v>1976</v>
       </c>
-      <c r="B52" s="44">
+      <c r="B52" s="43">
         <v>35</v>
       </c>
       <c r="C52" s="21">
@@ -7833,7 +8622,7 @@
         <f t="shared" si="9"/>
         <v>1976</v>
       </c>
-      <c r="B53" s="44">
+      <c r="B53" s="43">
         <v>36</v>
       </c>
       <c r="C53" s="21">
@@ -7884,21 +8673,21 @@
         <f t="shared" si="9"/>
         <v>1976</v>
       </c>
-      <c r="B54" s="45">
+      <c r="B54" s="44">
         <v>37</v>
       </c>
-      <c r="C54" s="46">
+      <c r="C54" s="45">
         <v>139.22200000000001</v>
       </c>
-      <c r="D54" s="47">
+      <c r="D54" s="46">
         <f t="shared" si="0"/>
         <v>144.86623006518442</v>
       </c>
-      <c r="E54" s="48">
+      <c r="E54" s="47">
         <f t="shared" si="1"/>
         <v>2.2557485084678475</v>
       </c>
-      <c r="F54" s="48">
+      <c r="F54" s="47">
         <f t="shared" si="2"/>
         <v>-27.782988067742778</v>
       </c>
@@ -7906,7 +8695,7 @@
         <f t="shared" si="3"/>
         <v>161.36075800255838</v>
       </c>
-      <c r="H54" s="46">
+      <c r="H54" s="45">
         <v>1</v>
       </c>
       <c r="I54" s="16">
@@ -7917,7 +8706,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K54" s="46">
+      <c r="K54" s="45">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
@@ -7935,41 +8724,41 @@
         <f t="shared" si="9"/>
         <v>1977</v>
       </c>
-      <c r="B55" s="49">
+      <c r="B55" s="48">
         <v>38</v>
       </c>
-      <c r="C55" s="50">
+      <c r="C55" s="49">
         <f>G54</f>
         <v>161.36075800255838</v>
       </c>
-      <c r="D55" s="51"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="53">
+      <c r="D55" s="50"/>
+      <c r="E55" s="51"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="52">
         <f>$D$54+H55*($E$54)+F51</f>
         <v>142.47899495718772</v>
       </c>
-      <c r="H55" s="49">
-        <v>1</v>
-      </c>
-      <c r="I55" s="54"/>
-      <c r="J55" s="49">
+      <c r="H55" s="48">
+        <v>1</v>
+      </c>
+      <c r="I55" s="53"/>
+      <c r="J55" s="48">
         <f>INT((H55-1)/$G$4)</f>
         <v>0</v>
       </c>
-      <c r="K55" s="49">
+      <c r="K55" s="48">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="L55" s="49">
+      <c r="L55" s="48">
         <f>$B$54+H55-K55</f>
         <v>34</v>
       </c>
-      <c r="M55" s="55">
+      <c r="M55" s="54">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="N55" s="60" t="s">
+      <c r="N55" s="59" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7978,328 +8767,328 @@
         <f t="shared" si="9"/>
         <v>1977</v>
       </c>
-      <c r="B56" s="49">
+      <c r="B56" s="48">
         <v>39</v>
       </c>
-      <c r="C56" s="50">
+      <c r="C56" s="49">
         <f>G55</f>
         <v>142.47899495718772</v>
       </c>
-      <c r="D56" s="51"/>
-      <c r="E56" s="52"/>
-      <c r="F56" s="52"/>
-      <c r="G56" s="53">
+      <c r="D56" s="50"/>
+      <c r="E56" s="51"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="52">
         <f>$D$54+H56*($E$54)+F52</f>
         <v>145.73319392553856</v>
       </c>
-      <c r="H56" s="49">
+      <c r="H56" s="48">
         <v>2</v>
       </c>
-      <c r="I56" s="54"/>
-      <c r="J56" s="49">
+      <c r="I56" s="53"/>
+      <c r="J56" s="48">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K56" s="49">
+      <c r="K56" s="48">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="L56" s="49">
+      <c r="L56" s="48">
         <f>$B$54+H56-K56</f>
         <v>35</v>
       </c>
-      <c r="M56" s="55">
+      <c r="M56" s="54">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="N56" s="61"/>
+      <c r="N56" s="60"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="18">
         <f t="shared" si="9"/>
         <v>1977</v>
       </c>
-      <c r="B57" s="49">
+      <c r="B57" s="48">
         <v>40</v>
       </c>
-      <c r="C57" s="50">
+      <c r="C57" s="49">
         <f>G56</f>
         <v>145.73319392553856</v>
       </c>
-      <c r="D57" s="51"/>
-      <c r="E57" s="52"/>
-      <c r="F57" s="52"/>
-      <c r="G57" s="53">
+      <c r="D57" s="50"/>
+      <c r="E57" s="51"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="52">
         <f>$D$54+H57*($E$54)+F53</f>
         <v>276.33990772148434</v>
       </c>
-      <c r="H57" s="49">
+      <c r="H57" s="48">
         <v>3</v>
       </c>
-      <c r="I57" s="54"/>
-      <c r="J57" s="49">
+      <c r="I57" s="53"/>
+      <c r="J57" s="48">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K57" s="49">
+      <c r="K57" s="48">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="L57" s="49">
+      <c r="L57" s="48">
         <f t="shared" ref="L57:L58" si="10">$B$54+H57-K57</f>
         <v>36</v>
       </c>
-      <c r="M57" s="55">
+      <c r="M57" s="54">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="N57" s="61"/>
+      <c r="N57" s="60"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="18">
         <f t="shared" si="9"/>
         <v>1977</v>
       </c>
-      <c r="B58" s="49">
+      <c r="B58" s="48">
         <v>41</v>
       </c>
-      <c r="C58" s="50">
+      <c r="C58" s="49">
         <f t="shared" ref="C58:C59" si="11">G57</f>
         <v>276.33990772148434</v>
       </c>
-      <c r="D58" s="51"/>
-      <c r="E58" s="52"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="53">
+      <c r="D58" s="50"/>
+      <c r="E58" s="51"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="52">
         <f>$D$54+H58*($E$54)+F54</f>
         <v>126.10623603131303</v>
       </c>
-      <c r="H58" s="49">
-        <v>4</v>
-      </c>
-      <c r="I58" s="54"/>
-      <c r="J58" s="49">
+      <c r="H58" s="48">
+        <v>4</v>
+      </c>
+      <c r="I58" s="53"/>
+      <c r="J58" s="48">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K58" s="49">
+      <c r="K58" s="48">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="L58" s="49">
+      <c r="L58" s="48">
         <f t="shared" si="10"/>
         <v>37</v>
       </c>
-      <c r="M58" s="55">
+      <c r="M58" s="54">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="N58" s="61"/>
+      <c r="N58" s="60"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="18">
         <f t="shared" si="9"/>
         <v>1978</v>
       </c>
-      <c r="B59" s="49">
+      <c r="B59" s="48">
         <v>42</v>
       </c>
-      <c r="C59" s="50">
+      <c r="C59" s="49">
         <f t="shared" si="11"/>
         <v>126.10623603131303</v>
       </c>
-      <c r="D59" s="51"/>
-      <c r="E59" s="52"/>
-      <c r="F59" s="52"/>
-      <c r="G59" s="53">
+      <c r="D59" s="50"/>
+      <c r="E59" s="51"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="52">
         <f>$D$54+H59*($E$54)+F51</f>
         <v>151.50198899105911</v>
       </c>
-      <c r="H59" s="49">
+      <c r="H59" s="48">
         <v>5</v>
       </c>
-      <c r="I59" s="54"/>
-      <c r="J59" s="49">
+      <c r="I59" s="53"/>
+      <c r="J59" s="48">
         <f>INT((H59-1)/$G$4)</f>
         <v>1</v>
       </c>
-      <c r="K59" s="49">
+      <c r="K59" s="48">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="L59" s="49">
+      <c r="L59" s="48">
         <f>$B$54+H59-K59</f>
         <v>34</v>
       </c>
-      <c r="M59" s="55">
+      <c r="M59" s="54">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="N59" s="61"/>
+      <c r="N59" s="60"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="18">
         <f t="shared" si="9"/>
         <v>1978</v>
       </c>
-      <c r="B60" s="49">
+      <c r="B60" s="48">
         <v>43</v>
       </c>
-      <c r="C60" s="50">
+      <c r="C60" s="49">
         <f>G59</f>
         <v>151.50198899105911</v>
       </c>
-      <c r="D60" s="51"/>
-      <c r="E60" s="52"/>
-      <c r="F60" s="52"/>
-      <c r="G60" s="53">
+      <c r="D60" s="50"/>
+      <c r="E60" s="51"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="52">
         <f t="shared" ref="G60:G62" si="12">$D$54+H60*($E$54)+F52</f>
         <v>154.75618795940994</v>
       </c>
-      <c r="H60" s="49">
+      <c r="H60" s="48">
         <v>6</v>
       </c>
-      <c r="I60" s="54"/>
-      <c r="J60" s="49">
+      <c r="I60" s="53"/>
+      <c r="J60" s="48">
         <f>INT((H60-1)/$G$4)</f>
         <v>1</v>
       </c>
-      <c r="K60" s="49">
+      <c r="K60" s="48">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="L60" s="49">
+      <c r="L60" s="48">
         <f>$B$54+H60-K60</f>
         <v>35</v>
       </c>
-      <c r="M60" s="55">
+      <c r="M60" s="54">
         <f t="shared" ref="M60:M63" si="13">B60-L60</f>
         <v>8</v>
       </c>
-      <c r="N60" s="61"/>
+      <c r="N60" s="60"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
         <f t="shared" si="9"/>
         <v>1978</v>
       </c>
-      <c r="B61" s="49">
+      <c r="B61" s="48">
         <v>44</v>
       </c>
-      <c r="C61" s="50">
+      <c r="C61" s="49">
         <f>G60</f>
         <v>154.75618795940994</v>
       </c>
-      <c r="D61" s="51"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="53">
+      <c r="D61" s="50"/>
+      <c r="E61" s="51"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="52">
         <f t="shared" si="12"/>
         <v>285.36290175535572</v>
       </c>
-      <c r="H61" s="49">
+      <c r="H61" s="48">
         <v>7</v>
       </c>
-      <c r="I61" s="54"/>
-      <c r="J61" s="49">
+      <c r="I61" s="53"/>
+      <c r="J61" s="48">
         <f>INT((H61-1)/$G$4)</f>
         <v>1</v>
       </c>
-      <c r="K61" s="49">
+      <c r="K61" s="48">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="L61" s="49">
+      <c r="L61" s="48">
         <f>$B$54+H61-K61</f>
         <v>36</v>
       </c>
-      <c r="M61" s="55">
+      <c r="M61" s="54">
         <f t="shared" si="13"/>
         <v>8</v>
       </c>
-      <c r="N61" s="61"/>
+      <c r="N61" s="60"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="18">
         <f t="shared" si="9"/>
         <v>1978</v>
       </c>
-      <c r="B62" s="49">
+      <c r="B62" s="48">
         <v>45</v>
       </c>
-      <c r="C62" s="50">
+      <c r="C62" s="49">
         <f>G61</f>
         <v>285.36290175535572</v>
       </c>
-      <c r="D62" s="51"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="53">
+      <c r="D62" s="50"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="52">
         <f t="shared" si="12"/>
         <v>135.1292300651844</v>
       </c>
-      <c r="H62" s="49">
+      <c r="H62" s="48">
         <v>8</v>
       </c>
-      <c r="I62" s="54"/>
-      <c r="J62" s="49">
+      <c r="I62" s="53"/>
+      <c r="J62" s="48">
         <f>INT((H62-1)/$G$4)</f>
         <v>1</v>
       </c>
-      <c r="K62" s="49">
+      <c r="K62" s="48">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="L62" s="49">
+      <c r="L62" s="48">
         <f>$B$54+H62-K62</f>
         <v>37</v>
       </c>
-      <c r="M62" s="55">
+      <c r="M62" s="54">
         <f t="shared" si="13"/>
         <v>8</v>
       </c>
-      <c r="N62" s="61"/>
+      <c r="N62" s="60"/>
     </row>
     <row r="63" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18">
         <f t="shared" si="9"/>
         <v>1979</v>
       </c>
-      <c r="B63" s="49">
+      <c r="B63" s="48">
         <v>46</v>
       </c>
-      <c r="C63" s="50">
+      <c r="C63" s="49">
         <f>G62</f>
         <v>135.1292300651844</v>
       </c>
-      <c r="D63" s="51"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="53">
+      <c r="D63" s="50"/>
+      <c r="E63" s="51"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="52">
         <f>$D$54+H63*($E$54)+F51</f>
         <v>160.52498302493049</v>
       </c>
-      <c r="H63" s="49">
+      <c r="H63" s="48">
         <v>9</v>
       </c>
-      <c r="I63" s="54"/>
-      <c r="J63" s="49">
+      <c r="I63" s="53"/>
+      <c r="J63" s="48">
         <f>INT((H63-1)/$G$4)</f>
         <v>2</v>
       </c>
-      <c r="K63" s="49">
+      <c r="K63" s="48">
         <f>$G$4*(J63+1)</f>
         <v>12</v>
       </c>
-      <c r="L63" s="49">
+      <c r="L63" s="48">
         <f>$B$54+H63-K63</f>
         <v>34</v>
       </c>
-      <c r="M63" s="55">
+      <c r="M63" s="54">
         <f t="shared" si="13"/>
         <v>12</v>
       </c>
-      <c r="N63" s="62"/>
+      <c r="N63" s="61"/>
     </row>
     <row r="67" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J67" s="7">

</xml_diff>